<commit_message>
Created basic frame types and ability for reader to create these frame objects from excel sheet
</commit_message>
<xml_diff>
--- a/docs/example configurations/1553Config.xlsx
+++ b/docs/example configurations/1553Config.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjacobso\Desktop\SCM\1553-Configurator\docs\example configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42835F00-3786-41D9-B1FD-9E0C8A513CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A8B6C5-339F-4DCD-ABE5-975160D23D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35235" yWindow="1215" windowWidth="21600" windowHeight="11385" xr2:uid="{1D4A689B-7892-44FC-B42C-AFEBC0BB0B5B}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{1D4A689B-7892-44FC-B42C-AFEBC0BB0B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="4" r:id="rId1"/>
     <sheet name="Parameters" sheetId="5" r:id="rId2"/>
-    <sheet name="MinorFrames" sheetId="6" r:id="rId3"/>
+    <sheet name="Frames" sheetId="6" r:id="rId3"/>
     <sheet name="All Info" sheetId="1" r:id="rId4"/>
     <sheet name="Reduced Info" sheetId="2" r:id="rId5"/>
     <sheet name="Minimal Info" sheetId="3" r:id="rId6"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="158">
   <si>
     <t>coreConfiguration</t>
   </si>
@@ -463,39 +463,6 @@
     <t>SA</t>
   </si>
   <si>
-    <t>Message 1</t>
-  </si>
-  <si>
-    <t>message 2</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
-    <t>OtherMEssage</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Items</t>
-  </si>
-  <si>
-    <t>100u</t>
-  </si>
-  <si>
-    <t>Minor 1</t>
-  </si>
-  <si>
-    <t>Minor 2</t>
-  </si>
-  <si>
-    <t>Acyclic 1</t>
-  </si>
-  <si>
     <t>BC to RT1 (SA2)</t>
   </si>
   <si>
@@ -533,6 +500,21 @@
   </si>
   <si>
     <t>words</t>
+  </si>
+  <si>
+    <t>MajorFrame1</t>
+  </si>
+  <si>
+    <t>MinorFrame1</t>
+  </si>
+  <si>
+    <t>MinorFrame2</t>
+  </si>
+  <si>
+    <t>AcyclicFrame</t>
+  </si>
+  <si>
+    <t>AcyclicFrame1</t>
   </si>
 </sst>
 </file>
@@ -572,10 +554,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF24292F"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -586,7 +569,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -613,26 +596,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -643,11 +606,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -662,12 +636,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -984,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76481921-E642-4285-ACC9-390C3589DAA0}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +988,7 @@
         <v>49</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>51</v>
@@ -1031,11 +1004,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>151</v>
+      <c r="A2" s="11" t="s">
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1049,10 +1022,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -1066,10 +1039,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1083,10 +1056,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C5">
         <v>15</v>
@@ -1100,10 +1073,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -1123,10 +1096,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1146,7 +1119,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
@@ -1164,12 +1137,12 @@
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
         <v>62</v>
@@ -1353,140 +1326,124 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D986984B-255F-49B4-A772-B8023AE31745}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12">
+        <v>100</v>
+      </c>
+      <c r="C2" s="12">
+        <v>200</v>
+      </c>
+      <c r="D2" s="12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="C4" t="s">
         <v>146</v>
       </c>
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>

</xml_diff>

<commit_message>
major and minor frames to bti 1553 xml
</commit_message>
<xml_diff>
--- a/docs/example configurations/1553Config.xlsx
+++ b/docs/example configurations/1553Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjacobso\Desktop\SCM\1553-Configurator\docs\example configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A8B6C5-339F-4DCD-ABE5-975160D23D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6A8956-062C-49FD-807D-8C2B32B1A629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{1D4A689B-7892-44FC-B42C-AFEBC0BB0B5B}"/>
+    <workbookView xWindow="4260" yWindow="2205" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{1D4A689B-7892-44FC-B42C-AFEBC0BB0B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="157">
   <si>
     <t>coreConfiguration</t>
   </si>
@@ -509,9 +509,6 @@
   </si>
   <si>
     <t>MinorFrame2</t>
-  </si>
-  <si>
-    <t>AcyclicFrame</t>
   </si>
   <si>
     <t>AcyclicFrame1</t>
@@ -621,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -638,7 +635,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
@@ -957,9 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76481921-E642-4285-ACC9-390C3589DAA0}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1004,7 +998,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>140</v>
       </c>
       <c r="B2" t="s">
@@ -1326,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D986984B-255F-49B4-A772-B8023AE31745}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1352,18 +1346,18 @@
         <v>155</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11">
         <v>100</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>200</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>-1</v>
       </c>
     </row>
@@ -1371,7 +1365,7 @@
       <c r="A3" t="s">
         <v>154</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>140</v>
       </c>
       <c r="C3" t="s">
@@ -1394,59 +1388,11 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added rermote terminal generation for hardware xml
</commit_message>
<xml_diff>
--- a/docs/example configurations/1553Config.xlsx
+++ b/docs/example configurations/1553Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjacobso\Desktop\SCM\1553-Configurator\docs\example configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6A8956-062C-49FD-807D-8C2B32B1A629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959E62BF-8F09-4B93-AF4B-4097E99D4415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2205" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{1D4A689B-7892-44FC-B42C-AFEBC0BB0B5B}"/>
+    <workbookView xWindow="30255" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{1D4A689B-7892-44FC-B42C-AFEBC0BB0B5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="157">
   <si>
     <t>coreConfiguration</t>
   </si>
@@ -618,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -637,6 +637,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,15 +954,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76481921-E642-4285-ACC9-390C3589DAA0}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -1107,7 +1110,7 @@
       <c r="F7">
         <v>15</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="12">
         <v>21</v>
       </c>
     </row>
@@ -1322,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D986984B-255F-49B4-A772-B8023AE31745}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,6 +1395,9 @@
       </c>
       <c r="B5" t="s">
         <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>